<commit_message>
feat: update styles, fixed header
</commit_message>
<xml_diff>
--- a/assets/students.xlsx
+++ b/assets/students.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2901" uniqueCount="1069">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2898" uniqueCount="1069">
   <si>
     <t/>
   </si>
@@ -3245,12 +3245,17 @@
       <name val="Times New Roman"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="40E0D0"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -3268,11 +3273,11 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3613,147 +3618,138 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI127"/>
+  <dimension ref="A1:AJ127"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="1" width="13.571428571428571" customWidth="1"/>
-    <col min="2" max="2" width="27.285714285714285" customWidth="1"/>
-    <col min="3" max="3" width="16.571428571428573" customWidth="1"/>
-    <col min="4" max="5" width="12.714285714285714" customWidth="1"/>
-    <col min="6" max="6" width="13.857142857142858" customWidth="1"/>
-    <col min="7" max="7" width="16.285714285714285" customWidth="1"/>
-    <col min="8" max="8" width="12.714285714285714" customWidth="1"/>
-    <col min="9" max="9" width="14.571428571428571" customWidth="1"/>
-    <col min="10" max="10" width="16" customWidth="1"/>
-    <col min="11" max="11" width="13.571428571428571" customWidth="1"/>
-    <col min="12" max="12" width="7.428571428571429" customWidth="1"/>
-    <col min="13" max="13" width="18.571428571428573" customWidth="1"/>
-    <col min="14" max="14" width="12.571428571428571" customWidth="1"/>
-    <col min="15" max="15" width="15.571428571428571" customWidth="1"/>
-    <col min="16" max="16" width="29.142857142857142" customWidth="1"/>
-    <col min="17" max="17" width="38.42857142857143" customWidth="1"/>
-    <col min="18" max="18" width="23.142857142857142" customWidth="1"/>
-    <col min="19" max="19" width="15.285714285714286" customWidth="1"/>
-    <col min="20" max="20" width="15.571428571428571" customWidth="1"/>
-    <col min="21" max="21" width="13.571428571428571" customWidth="1"/>
-    <col min="22" max="22" width="17.714285714285715" customWidth="1"/>
-    <col min="23" max="23" width="24.857142857142858" customWidth="1"/>
-    <col min="24" max="24" width="17.428571428571427" customWidth="1"/>
-    <col min="25" max="25" width="24.714285714285715" customWidth="1"/>
-    <col min="26" max="26" width="30.857142857142858" customWidth="1"/>
-    <col min="27" max="28" width="11" customWidth="1"/>
-    <col min="29" max="29" width="7" customWidth="1"/>
-    <col min="30" max="30" width="11" customWidth="1"/>
+    <col min="1" max="1" width="6" customWidth="1"/>
+    <col min="2" max="3" width="35" customWidth="1"/>
+    <col min="4" max="5" width="16" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
+    <col min="7" max="7" width="21" customWidth="1"/>
+    <col min="8" max="8" width="14" customWidth="1"/>
+    <col min="9" max="9" width="45" customWidth="1"/>
+    <col min="10" max="10" width="20" customWidth="1"/>
+    <col min="11" max="11" width="15" customWidth="1"/>
+    <col min="12" max="12" width="8" customWidth="1"/>
+    <col min="13" max="13" width="23" customWidth="1"/>
+    <col min="14" max="14" width="20" customWidth="1"/>
+    <col min="15" max="15" width="30" customWidth="1"/>
+    <col min="16" max="16" width="7" customWidth="1"/>
+    <col min="17" max="18" width="10" customWidth="1"/>
+    <col min="19" max="19" width="7" customWidth="1"/>
+    <col min="20" max="21" width="10" customWidth="1"/>
+    <col min="22" max="22" width="51" customWidth="1"/>
+    <col min="23" max="23" width="21" customWidth="1"/>
+    <col min="24" max="25" width="16" customWidth="1"/>
+    <col min="26" max="26" width="33" customWidth="1"/>
+    <col min="27" max="27" width="21" customWidth="1"/>
+    <col min="28" max="29" width="22" customWidth="1"/>
+    <col min="30" max="30" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L1" t="s">
-        <v>0</v>
-      </c>
-      <c r="M1" t="s">
-        <v>0</v>
-      </c>
-      <c r="N1" t="s">
-        <v>0</v>
-      </c>
-      <c r="O1" t="s">
-        <v>0</v>
-      </c>
-      <c r="P1" t="s">
+    <row r="1" ht="90" customHeight="1" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Q1" t="s">
-        <v>0</v>
-      </c>
-      <c r="R1" t="s">
-        <v>0</v>
-      </c>
-      <c r="S1" t="s">
-        <v>0</v>
-      </c>
-      <c r="T1" t="s">
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="U1" t="s">
-        <v>0</v>
-      </c>
-      <c r="V1" t="s">
-        <v>0</v>
-      </c>
-      <c r="W1" t="s">
-        <v>0</v>
-      </c>
-      <c r="X1" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AI1" t="s">
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AJ1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" ht="49.333333333333336" customHeight="1" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" ht="90" customHeight="1" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -3845,7 +3841,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" ht="49.333333333333336" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -3937,7 +3933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" ht="61.333333333333336" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -4029,7 +4025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" ht="61.333333333333336" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -4121,7 +4117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" ht="61.333333333333336" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -4213,7 +4209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -4305,7 +4301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="8" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -4397,7 +4393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" ht="61.333333333333336" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="9" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -4489,7 +4485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="10" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -4581,7 +4577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" ht="73.33333333333333" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -4673,7 +4669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="12" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>10</v>
       </c>
@@ -4765,7 +4761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="13" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>11</v>
       </c>
@@ -4857,7 +4853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="14" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>12</v>
       </c>
@@ -4949,7 +4945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="15" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>13</v>
       </c>
@@ -5041,7 +5037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="16" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>14</v>
       </c>
@@ -5133,7 +5129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="17" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>15</v>
       </c>
@@ -5225,7 +5221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="18" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>16</v>
       </c>
@@ -5317,7 +5313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="19" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>17</v>
       </c>
@@ -5409,7 +5405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="20" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>18</v>
       </c>
@@ -5501,7 +5497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" ht="61.333333333333336" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="21" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>19</v>
       </c>
@@ -5593,7 +5589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" ht="61.333333333333336" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="22" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>20</v>
       </c>
@@ -5685,7 +5681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="23" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>21</v>
       </c>
@@ -5777,7 +5773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="24" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>22</v>
       </c>
@@ -5869,7 +5865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="25" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>23</v>
       </c>
@@ -5961,7 +5957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="26" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>24</v>
       </c>
@@ -6053,7 +6049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="27" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>25</v>
       </c>
@@ -6145,7 +6141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" ht="61.333333333333336" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="28" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>26</v>
       </c>
@@ -6237,7 +6233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="29" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>27</v>
       </c>
@@ -6329,7 +6325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="30" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>28</v>
       </c>
@@ -6421,7 +6417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="31" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>29</v>
       </c>
@@ -6513,7 +6509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="32" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>30</v>
       </c>
@@ -6605,7 +6601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" ht="61.333333333333336" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="33" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>31</v>
       </c>
@@ -6697,7 +6693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="34" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>32</v>
       </c>
@@ -6789,7 +6785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="35" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>33</v>
       </c>
@@ -6881,7 +6877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="36" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>34</v>
       </c>
@@ -6973,7 +6969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="37" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>35</v>
       </c>
@@ -7065,7 +7061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="38" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>36</v>
       </c>
@@ -7157,7 +7153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="39" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>37</v>
       </c>
@@ -7249,7 +7245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" ht="61.333333333333336" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="40" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>38</v>
       </c>
@@ -7341,7 +7337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="41" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>39</v>
       </c>
@@ -7433,7 +7429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="42" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>40</v>
       </c>
@@ -7525,7 +7521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="43" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>41</v>
       </c>
@@ -7617,7 +7613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="44" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>42</v>
       </c>
@@ -7709,7 +7705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="45" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>43</v>
       </c>
@@ -7801,7 +7797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="46" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>44</v>
       </c>
@@ -7893,7 +7889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="47" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>45</v>
       </c>
@@ -7985,7 +7981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="48" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>46</v>
       </c>
@@ -8077,7 +8073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="49" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>47</v>
       </c>
@@ -8169,7 +8165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="50" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>48</v>
       </c>
@@ -8261,7 +8257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="51" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>49</v>
       </c>
@@ -8353,7 +8349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="52" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>50</v>
       </c>
@@ -8445,7 +8441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="53" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>51</v>
       </c>
@@ -8537,7 +8533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="54" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>52</v>
       </c>
@@ -8629,7 +8625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="55" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>53</v>
       </c>
@@ -8721,7 +8717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="56" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>54</v>
       </c>
@@ -8813,7 +8809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="57" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>55</v>
       </c>
@@ -8905,7 +8901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="58" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>56</v>
       </c>
@@ -8997,7 +8993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="59" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>57</v>
       </c>
@@ -9089,7 +9085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="60" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>58</v>
       </c>
@@ -9181,7 +9177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="61" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>59</v>
       </c>
@@ -9273,7 +9269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="62" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>60</v>
       </c>
@@ -9365,7 +9361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="63" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>61</v>
       </c>
@@ -9457,7 +9453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="64" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
         <v>62</v>
       </c>
@@ -9549,7 +9545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="65" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>63</v>
       </c>
@@ -9641,7 +9637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="66" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <v>64</v>
       </c>
@@ -9733,7 +9729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="67" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>65</v>
       </c>
@@ -9825,7 +9821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="68" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
         <v>66</v>
       </c>
@@ -9917,7 +9913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="69" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
         <v>67</v>
       </c>
@@ -10009,7 +10005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="70" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
         <v>68</v>
       </c>
@@ -10101,7 +10097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="71" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
         <v>69</v>
       </c>
@@ -10193,7 +10189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="72" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
         <v>70</v>
       </c>
@@ -10285,7 +10281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="73" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
         <v>71</v>
       </c>
@@ -10377,7 +10373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="74" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
         <v>72</v>
       </c>
@@ -10469,7 +10465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="75" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
         <v>73</v>
       </c>
@@ -10561,7 +10557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="76" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
         <v>74</v>
       </c>
@@ -10653,7 +10649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="77" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
         <v>75</v>
       </c>
@@ -10745,7 +10741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="78" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
         <v>76</v>
       </c>
@@ -10837,7 +10833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="79" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
         <v>77</v>
       </c>
@@ -10929,7 +10925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="80" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
         <v>78</v>
       </c>
@@ -11021,7 +11017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="81" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
         <v>79</v>
       </c>
@@ -11113,7 +11109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="82" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
         <v>80</v>
       </c>
@@ -11205,7 +11201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="83" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
         <v>81</v>
       </c>
@@ -11297,7 +11293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="84" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A84" s="3">
         <v>82</v>
       </c>
@@ -11389,7 +11385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="85" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A85" s="3">
         <v>83</v>
       </c>
@@ -11481,7 +11477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="86" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A86" s="3">
         <v>84</v>
       </c>
@@ -11573,7 +11569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="87" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A87" s="3">
         <v>85</v>
       </c>
@@ -11665,7 +11661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="88" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A88" s="3">
         <v>86</v>
       </c>
@@ -11757,7 +11753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="89" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A89" s="3">
         <v>87</v>
       </c>
@@ -11849,7 +11845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="90" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A90" s="3">
         <v>88</v>
       </c>
@@ -11941,7 +11937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="91" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A91" s="3">
         <v>89</v>
       </c>
@@ -12033,7 +12029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="92" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A92" s="3">
         <v>90</v>
       </c>
@@ -12125,7 +12121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="93" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A93" s="3">
         <v>91</v>
       </c>
@@ -12217,7 +12213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="94" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A94" s="3">
         <v>92</v>
       </c>
@@ -12309,7 +12305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="95" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A95" s="3">
         <v>93</v>
       </c>
@@ -12401,7 +12397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" ht="86" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="96" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A96" s="3">
         <v>94</v>
       </c>
@@ -12493,7 +12489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" ht="86" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="97" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A97" s="3">
         <v>95</v>
       </c>
@@ -12585,7 +12581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="98" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A98" s="3">
         <v>96</v>
       </c>
@@ -12677,7 +12673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="99" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A99" s="3">
         <v>97</v>
       </c>
@@ -12769,7 +12765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="100" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A100" s="3">
         <v>98</v>
       </c>
@@ -12861,7 +12857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="101" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A101" s="3">
         <v>99</v>
       </c>
@@ -12953,7 +12949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" ht="61.333333333333336" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="102" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A102" s="3">
         <v>100</v>
       </c>
@@ -13045,7 +13041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" ht="61.333333333333336" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="103" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A103" s="3">
         <v>101</v>
       </c>
@@ -13137,7 +13133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="104" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A104" s="3">
         <v>102</v>
       </c>
@@ -13229,7 +13225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="105" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A105" s="3">
         <v>103</v>
       </c>
@@ -13321,7 +13317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="106" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A106" s="3">
         <v>104</v>
       </c>
@@ -13413,7 +13409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="107" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A107" s="3">
         <v>105</v>
       </c>
@@ -13505,7 +13501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="108" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A108" s="3">
         <v>106</v>
       </c>
@@ -13597,7 +13593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="109" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A109" s="3">
         <v>107</v>
       </c>
@@ -13689,7 +13685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="110" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A110" s="3">
         <v>108</v>
       </c>
@@ -13781,7 +13777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="111" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A111" s="3">
         <v>109</v>
       </c>
@@ -13873,7 +13869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="112" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A112" s="3">
         <v>110</v>
       </c>
@@ -13965,7 +13961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="113" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A113" s="3">
         <v>111</v>
       </c>
@@ -14057,7 +14053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="114" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A114" s="3">
         <v>112</v>
       </c>
@@ -14149,7 +14145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="115" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A115" s="3">
         <v>113</v>
       </c>
@@ -14241,7 +14237,7 @@
         <v>974</v>
       </c>
     </row>
-    <row r="116" ht="73.33333333333333" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="116" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A116" s="3">
         <v>114</v>
       </c>
@@ -14333,7 +14329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="117" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A117" s="3">
         <v>115</v>
       </c>
@@ -14425,7 +14421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="118" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A118" s="3">
         <v>116</v>
       </c>
@@ -14517,7 +14513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="119" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A119" s="3">
         <v>117</v>
       </c>
@@ -14609,7 +14605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="120" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A120" s="3">
         <v>118</v>
       </c>
@@ -14701,7 +14697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="121" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A121" s="3">
         <v>119</v>
       </c>
@@ -14793,7 +14789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="122" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A122" s="3">
         <v>120</v>
       </c>
@@ -14885,7 +14881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" ht="73.33333333333333" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="123" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A123" s="3">
         <v>121</v>
       </c>
@@ -14977,7 +14973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" ht="73.33333333333333" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="124" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A124" s="3">
         <v>122</v>
       </c>
@@ -15069,7 +15065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" ht="48.666666666666664" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="125" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A125" s="3">
         <v>123</v>
       </c>
@@ -15161,7 +15157,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" ht="48.666666666666664" customHeight="1" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="126" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A126" s="3">
+        <v>124</v>
+      </c>
       <c r="B126" s="3" t="s">
         <v>1053</v>
       </c>
@@ -15250,7 +15249,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" ht="61.333333333333336" customHeight="1" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="127" ht="90" customHeight="1" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A127" s="3">
+        <v>125</v>
+      </c>
       <c r="B127" s="3" t="s">
         <v>1062</v>
       </c>
@@ -15340,6 +15342,10 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="S1:U1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>

</xml_diff>